<commit_message>
2024-10-13 @ 08:36 - v4.K.3.xlsb
* modAppli.bas
   - Nouvelle variable globale pour contrôler la facturation (flagEtapeFacture)
* modFAC_Finale.bas
   - Meilleur contrôle du format de papier (lettre)
   - Enlever du code en commentaire
* ufListeProjetsFacture.frm
   - Ajustements esthétiques au listBox
* wshFAC_Brouillon.docccls
   - Executer à chaque fois la procédure _Activate
</commit_message>
<xml_diff>
--- a/Factures_Excel/1699 - An-Au Construction Inc.xlsx
+++ b/Factures_Excel/1699 - An-Au Construction Inc.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VBA\GC_FISCALITÉ\Factures_Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Administration\Facturation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2E604E0-D69F-4B27-92BF-BCD8940695EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B88E157-2795-4BE3-B5B9-AC4FC7427935}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="04-10-23" sheetId="4" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="11-05-24" sheetId="7" r:id="rId3"/>
     <sheet name="20-08-24" sheetId="8" r:id="rId4"/>
     <sheet name="Activités" sheetId="5" r:id="rId5"/>
-    <sheet name="2024-09-03 - 24-24481" sheetId="9" r:id="rId6"/>
+    <sheet name=" - 24-24481" sheetId="9" r:id="rId6"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId7"/>
@@ -291,6 +291,9 @@
     <t xml:space="preserve"> - Préparation des 8 formulaires de roulement T2057 et TP-518 requis;</t>
   </si>
   <si>
+    <t>Le 4 SEPTEMBRE 2024</t>
+  </si>
+  <si>
     <t>Patrick Michaud</t>
   </si>
   <si>
@@ -304,9 +307,6 @@
   </si>
   <si>
     <t>24-24481</t>
-  </si>
-  <si>
-    <t>Le 3 SEPTEMBRE 2024</t>
   </si>
   <si>
     <t>Frais d'expert en taxes</t>
@@ -326,7 +326,7 @@
     <numFmt numFmtId="168" formatCode="#,##0.00\ &quot;$&quot;"/>
     <numFmt numFmtId="169" formatCode="##0.00"/>
   </numFmts>
-  <fonts count="46" x14ac:knownFonts="1">
+  <fonts count="47" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -558,6 +558,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -1116,10 +1122,10 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="3" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="169" fontId="12" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="36" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="12" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="36" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="7" fontId="29" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1128,20 +1134,20 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="3" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="3" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="168" fontId="16" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="38" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="39" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -1163,22 +1169,22 @@
     </xf>
     <xf numFmtId="168" fontId="17" fillId="0" borderId="17" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="168" fontId="37" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="38" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="166" fontId="17" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="168" fontId="16" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="16" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="168" fontId="17" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1206,20 +1212,20 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
@@ -1234,10 +1240,10 @@
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1249,7 +1255,7 @@
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Milliers" xfId="1" builtinId="3"/>
-    <cellStyle name="Milliers 2" xfId="5" xr:uid="{A4E7B80E-2016-4FD6-A0EA-628A305F914F}"/>
+    <cellStyle name="Milliers 2" xfId="5" xr:uid="{055F9840-EBA2-4AA7-9377-311F5B890732}"/>
     <cellStyle name="Monétaire" xfId="2" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="3" xr:uid="{05AE08AC-AFEC-4B9B-A8E8-E482E13645AE}"/>
@@ -1580,7 +1586,7 @@
         <xdr:cNvPr id="2" name="GCF_Entête" descr="Une image contenant texte, capture d’écran, Police, conception&#10;&#10;Description générée automatiquement">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{585AF239-AD3F-4E8A-A0F7-F82F39E97E79}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF646905-3935-4FF6-86B8-E27907886662}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1622,7 +1628,9 @@
       <xxl21:absoluteUrl r:id="rId2"/>
     </xxl21:alternateUrls>
     <sheetNames>
+      <sheetName val="Doc_Search_Utility_Results"/>
       <sheetName val="X_Analyse_Intégrité"/>
+      <sheetName val="X_Heures_Jour_Prof"/>
       <sheetName val="Menu"/>
       <sheetName val="Admin"/>
       <sheetName val="BD_Clients"/>
@@ -1657,7 +1665,7 @@
       <sheetName val="GL_EJ_Auto"/>
       <sheetName val="GL_Rapport"/>
       <sheetName val="GL_Trans"/>
-      <sheetName val="HresJourProf"/>
+      <sheetName val="Hres_Jour_Prof"/>
       <sheetName val="MenuDEB"/>
       <sheetName val="MenuFACT"/>
       <sheetName val="MenuGL"/>
@@ -1665,15 +1673,17 @@
       <sheetName val="TEC_Analyse"/>
       <sheetName val="TEC_TDB"/>
       <sheetName val="TEC_TDB_Data"/>
-      <sheetName val="CAR_TDB_Data"/>
-      <sheetName val="CAR_TDB_PivotTable"/>
       <sheetName val="TEC_TDB_PivotTable"/>
       <sheetName val="TEC_Local"/>
+      <sheetName val="zCAR_TDB_Data"/>
+      <sheetName val="zCAR_TDB_PivotTable"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
       <sheetData sheetId="1"/>
-      <sheetData sheetId="2">
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4">
         <row r="10">
           <cell r="Z10" t="str">
             <v>Description</v>
@@ -1900,8 +1910,6 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
       <sheetData sheetId="5"/>
       <sheetData sheetId="6"/>
       <sheetData sheetId="7"/>
@@ -1944,6 +1952,8 @@
       <sheetData sheetId="44"/>
       <sheetData sheetId="45"/>
       <sheetData sheetId="46"/>
+      <sheetData sheetId="47"/>
+      <sheetData sheetId="48"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -3007,7 +3017,7 @@
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
-  <pageSetup paperSize="131" scale="33" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup paperSize="131" scale="62" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <headerFooter scaleWithDoc="0" alignWithMargins="0"/>
   <drawing r:id="rId2"/>
 </worksheet>
@@ -3759,7 +3769,7 @@
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
-  <pageSetup paperSize="131" scale="33" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup paperSize="131" scale="62" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <headerFooter scaleWithDoc="0" alignWithMargins="0"/>
   <drawing r:id="rId2"/>
 </worksheet>
@@ -4535,7 +4545,7 @@
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
-  <pageSetup paperSize="131" scale="33" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup paperSize="131" scale="62" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <headerFooter scaleWithDoc="0" alignWithMargins="0"/>
   <drawing r:id="rId2"/>
 </worksheet>
@@ -5295,7 +5305,7 @@
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
-  <pageSetup paperSize="131" scale="33" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup paperSize="131" scale="62" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <headerFooter scaleWithDoc="0" alignWithMargins="0"/>
   <drawing r:id="rId2"/>
 </worksheet>
@@ -5690,13 +5700,13 @@
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.4921259845" footer="0.4921259845"/>
-  <pageSetup scale="65" orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="74" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B66728E-E280-4851-80D6-D233A5D6DBBC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{281F14CC-7AF6-47AE-8A03-85E6A649567C}">
   <dimension ref="A1:F89"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -5874,7 +5884,7 @@
     <row r="21" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" s="70"/>
       <c r="B21" s="71" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C21" s="71"/>
       <c r="D21" s="72"/>
@@ -5892,7 +5902,7 @@
     <row r="23" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A23" s="70"/>
       <c r="B23" s="71" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C23" s="71"/>
       <c r="D23" s="72"/>
@@ -5902,7 +5912,7 @@
     <row r="24" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A24" s="70"/>
       <c r="B24" s="75" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C24" s="74"/>
       <c r="D24" s="72"/>
@@ -5912,7 +5922,7 @@
     <row r="25" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A25" s="70"/>
       <c r="B25" s="74" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C25" s="74"/>
       <c r="D25" s="72"/>
@@ -5922,7 +5932,7 @@
     <row r="26" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A26" s="70"/>
       <c r="B26" s="74" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C26" s="74"/>
       <c r="D26" s="72"/>
@@ -5945,7 +5955,7 @@
         <v>11</v>
       </c>
       <c r="E28" s="79" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F28" s="79"/>
     </row>
@@ -6522,10 +6532,10 @@
     <mergeCell ref="A88:F88"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" operator="lessThan" allowBlank="1" showInputMessage="1" sqref="B34 B36 B38" xr:uid="{BD731AFB-A5E2-42F9-A8F3-643C6B30B144}">
+    <dataValidation type="list" operator="lessThan" allowBlank="1" showInputMessage="1" sqref="B34 B36 B38" xr:uid="{F2679C1A-7035-496F-B29C-5B655FC28339}">
       <formula1>dnrServices</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B80:C80 B12:C20 B78:C78" xr:uid="{189CAF68-645F-4749-8278-CF05560E8F3A}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B80:C80 B12:C20 B78:C78" xr:uid="{549A8050-FFD7-438E-94D6-14FCD8054F00}">
       <formula1>Liste_Activités</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>